<commit_message>
Modify Test suite (Positive TCs) - automationpractice.xlsx after removing technical errors in some test cases
</commit_message>
<xml_diff>
--- a/AlexanderA/automationpractice.com/Test suite (Positive TCs) - automationpractice.xlsx
+++ b/AlexanderA/automationpractice.com/Test suite (Positive TCs) - automationpractice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="578">
   <si>
     <t xml:space="preserve">AUTOMATIONPRACTICE.COM TEST SUITE – POSITIVE TEST CASES</t>
   </si>
@@ -664,6 +664,9 @@
     <t xml:space="preserve">28. Check the “Terms and Conditions” checkbox and click on “Proceed to checkout” button</t>
   </si>
   <si>
+    <t xml:space="preserve">Load the fifth page (Payment page) from the order procedure. The quantities of the products are shown in “cart_summary” table (the quantity of the first product is 1 and the quantity of the second product is 1000)</t>
+  </si>
+  <si>
     <t xml:space="preserve">29. Click on “Pay by bank wire” link</t>
   </si>
   <si>
@@ -766,13 +769,13 @@
     <t xml:space="preserve">16. Select “Reference: Lowest first” from “Sort by” drop-down list</t>
   </si>
   <si>
-    <t xml:space="preserve">The items with the lowest references are showed before the other items</t>
+    <t xml:space="preserve">The items with the lowest references are shown before the other items</t>
   </si>
   <si>
     <t xml:space="preserve">17. Select “Reference: Highest first” from “Sort by” drop-down list</t>
   </si>
   <si>
-    <t xml:space="preserve">The items with the highest references are showed before the other items</t>
+    <t xml:space="preserve">The items with the highest references are shown before the other items</t>
   </si>
   <si>
     <t xml:space="preserve">18. Check “Dresses” checkbox </t>
@@ -856,7 +859,7 @@
     <t xml:space="preserve">6. Hover over the right side of the image first and then hover over the left side</t>
   </si>
   <si>
-    <t xml:space="preserve">A right arrow appears in the right area of the image first and after the position of the cursor is changed to the left side of the image a left arrow appears there</t>
+    <t xml:space="preserve">A right arrow appears in the right area of the image first and after the mouse cursor is moved to the left side of the image a left arrow appears there</t>
   </si>
   <si>
     <t xml:space="preserve">7. Click on the right area of the image</t>
@@ -991,7 +994,10 @@
     <t xml:space="preserve">4. Click on the “More” button under the image of another product</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Increase the quantity of the product by 100 and click on the “Add to cart” button</t>
+    <t xml:space="preserve">5. Increase the quantity of the product to 100 and click on the “Add to cart” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A dialog window with two buttons (“Continue shopping” and “Proceed to checkout”) appears. The following text is displayed: “Product successfully added to your cart. There are 101 item in your cart.”</t>
   </si>
   <si>
     <t xml:space="preserve">6. Click on “Continue shopping” button</t>
@@ -1195,27 +1201,24 @@
     <t xml:space="preserve">7. Type “TheseAreJustThirtyThreeCharactersTheseAreJustThirtyThreeCharactersTheseAreJustThirtyThreeCharacters,01234567890123456789,0123456” in “Address” field</t>
   </si>
   <si>
-    <t xml:space="preserve">None or the “Address” field becomes red and the input followed by “X” (fail sign) is displayed (Bug or Feature?) </t>
+    <t xml:space="preserve">The input is shown in the text field</t>
   </si>
   <si>
     <t xml:space="preserve">8. Type “AtextWithJustThirtyTwoCharactersAtextWithJustThirtyTwoCharacters” in “City” field</t>
   </si>
   <si>
-    <t xml:space="preserve">None or the “City” field becomes red and the input followed by “X” (fail sign) is displayed (Bug or Feature?) </t>
-  </si>
-  <si>
     <t xml:space="preserve">9. Choose Alabama as a state</t>
   </si>
   <si>
+    <t xml:space="preserve">The Alabama State is selected</t>
+  </si>
+  <si>
     <t xml:space="preserve">10. Type “99999” in “Zip/Postal code” field</t>
   </si>
   <si>
     <t xml:space="preserve">11. Type “01234567890123456789012345678901” in “Mobile phone” field</t>
   </si>
   <si>
-    <t xml:space="preserve">None or the “Mobile phone” field becomes red and the input followed by “X” (fail sign) is displayed (Bug or Feature?) </t>
-  </si>
-  <si>
     <t xml:space="preserve">12. Click on “Register” button</t>
   </si>
   <si>
@@ -1234,7 +1237,7 @@
     <t xml:space="preserve">Load a page containing all products from “Women” category</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Click on “Add to wishlist” link under the first product</t>
+    <t xml:space="preserve">5. Click on “Add to wishlist” link under the first product in the product list</t>
   </si>
   <si>
     <t xml:space="preserve">A fancybox appears. It contains the following text: “Added to your wishlist”</t>
@@ -1243,7 +1246,7 @@
     <t xml:space="preserve">6. Close the fancybox</t>
   </si>
   <si>
-    <t xml:space="preserve">7. Click on “Add to wishlist” link under the last product</t>
+    <t xml:space="preserve">7. Click on “Add to wishlist” link under the last product in the product list</t>
   </si>
   <si>
     <t xml:space="preserve">8. Close the fancybox</t>
@@ -1321,7 +1324,7 @@
     <t xml:space="preserve">12. Click on the “Compare” button</t>
   </si>
   <si>
-    <t xml:space="preserve">Load “Product comparison” page. The page includes information about the three products which were previously added for comparison</t>
+    <t xml:space="preserve">Load “Product comparison” page. The page includes information about the three products which were previously selected for comparison</t>
   </si>
   <si>
     <t xml:space="preserve">13. Click on the remove icon of the first product</t>
@@ -1778,7 +1781,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1839,6 +1842,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1918,7 +1927,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2023,6 +2032,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2114,16 +2127,16 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.8016194331984"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.8097165991903"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2418,16 +2431,16 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2472,7 +2485,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2480,7 +2493,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2515,7 +2528,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>89</v>
@@ -2523,7 +2536,7 @@
     </row>
     <row r="13" customFormat="false" ht="109" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>91</v>
@@ -2531,7 +2544,7 @@
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>95</v>
@@ -2539,7 +2552,7 @@
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>97</v>
@@ -2547,7 +2560,7 @@
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>99</v>
@@ -2555,50 +2568,50 @@
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="B18" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>389</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>391</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>391</v>
+        <v>392</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2622,16 +2635,16 @@
   </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2678,7 +2691,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2686,7 +2699,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2729,7 +2742,7 @@
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>176</v>
@@ -2737,47 +2750,47 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>176</v>
@@ -2785,58 +2798,58 @@
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2860,16 +2873,16 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2908,7 +2921,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,7 +2929,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +2937,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2967,7 +2980,7 @@
     </row>
     <row r="13" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>176</v>
@@ -2975,50 +2988,50 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3048,10 +3061,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3102,7 +3115,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,47 +3150,47 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>63</v>
@@ -3210,10 +3223,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3229,7 +3242,7 @@
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3264,7 +3277,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,7 +3312,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>63</v>
@@ -3307,10 +3320,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3345,10 +3358,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3364,7 +3377,7 @@
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3399,7 +3412,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3434,186 +3447,186 @@
     </row>
     <row r="12" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -3643,10 +3656,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3662,7 +3675,7 @@
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3697,7 +3710,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,15 +3745,15 @@
     </row>
     <row r="12" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>63</v>
@@ -3748,15 +3761,15 @@
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>63</v>
@@ -3764,15 +3777,15 @@
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>63</v>
@@ -3780,15 +3793,15 @@
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>63</v>
@@ -3796,15 +3809,15 @@
     </row>
     <row r="20" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>63</v>
@@ -3812,15 +3825,15 @@
     </row>
     <row r="22" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>63</v>
@@ -3828,15 +3841,15 @@
     </row>
     <row r="24" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>63</v>
@@ -3844,58 +3857,58 @@
     </row>
     <row r="26" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -3925,10 +3938,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -3979,7 +3992,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4014,98 +4027,98 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -4135,10 +4148,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4189,7 +4202,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4224,98 +4237,98 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="B15" s="27" t="s">
         <v>534</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
+        <v>536</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>535</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>536</v>
-      </c>
-      <c r="B17" s="27" t="s">
         <v>537</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
   </sheetData>
@@ -4345,10 +4358,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4364,7 +4377,7 @@
       <c r="A2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4399,7 +4412,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4428,120 +4441,120 @@
       <c r="A11" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="29" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="s">
-        <v>550</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="A12" s="29" t="s">
         <v>551</v>
       </c>
+      <c r="B12" s="29" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="s">
-        <v>552</v>
-      </c>
-      <c r="B13" s="28" t="s">
+      <c r="A13" s="29" t="s">
         <v>553</v>
       </c>
+      <c r="B13" s="29" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28" t="s">
-        <v>554</v>
-      </c>
-      <c r="B14" s="28" t="s">
+      <c r="A14" s="29" t="s">
         <v>555</v>
       </c>
+      <c r="B14" s="29" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28" t="s">
-        <v>556</v>
-      </c>
-      <c r="B15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>557</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>574</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
   </sheetData>
@@ -4565,16 +4578,16 @@
   </sheetPr>
   <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5103,16 +5116,16 @@
   </sheetPr>
   <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5413,20 +5426,20 @@
         <v>207</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>161</v>
@@ -5434,7 +5447,7 @@
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>176</v>
@@ -5442,7 +5455,7 @@
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>194</v>
@@ -5450,7 +5463,7 @@
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B43" s="11" t="s">
         <v>196</v>
@@ -5458,10 +5471,10 @@
     </row>
     <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -5560,16 +5573,16 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5620,7 +5633,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5655,231 +5668,231 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>65</v>
@@ -5887,7 +5900,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>67</v>
@@ -5895,10 +5908,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="11" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5922,16 +5935,16 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5976,7 +5989,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5984,7 +5997,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6019,15 +6032,15 @@
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>63</v>
@@ -6035,226 +6048,226 @@
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>275</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>279</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="11" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="11" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="11" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="11" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6282,15 +6295,15 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6341,7 +6354,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6371,12 +6384,12 @@
         <v>62</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>11</v>
@@ -6384,31 +6397,31 @@
     </row>
     <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>65</v>
+        <v>319</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>67</v>
@@ -6416,15 +6429,15 @@
     </row>
     <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>63</v>
@@ -6432,34 +6445,34 @@
     </row>
     <row r="19" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6490,10 +6503,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6544,7 +6557,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6579,26 +6592,26 @@
     </row>
     <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6633,10 +6646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6675,7 +6688,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6683,7 +6696,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6691,7 +6704,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6726,58 +6739,58 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -6801,16 +6814,16 @@
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="92.5506072874494"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6855,7 +6868,7 @@
         <v>55</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6898,7 +6911,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>89</v>
@@ -6906,7 +6919,7 @@
     </row>
     <row r="13" customFormat="false" ht="41.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>91</v>
@@ -6914,7 +6927,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>93</v>
@@ -6922,7 +6935,7 @@
     </row>
     <row r="15" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>95</v>
@@ -6930,7 +6943,7 @@
     </row>
     <row r="16" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>97</v>
@@ -6938,7 +6951,7 @@
     </row>
     <row r="17" customFormat="false" ht="28.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>99</v>
@@ -6946,7 +6959,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>101</v>
@@ -6954,7 +6967,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>103</v>
@@ -6962,7 +6975,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>103</v>
@@ -6970,71 +6983,71 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>176</v>

</xml_diff>